<commit_message>
Update Excel and Documents.
</commit_message>
<xml_diff>
--- a/InventoryTracker-WebApp/ExcelFiles/EntityEquipmentAssignDateRangeSample.xlsx
+++ b/InventoryTracker-WebApp/ExcelFiles/EntityEquipmentAssignDateRangeSample.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\IT For Publish\InventoryTracker\InventoryTracker-WebApp\ExcelFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\IT For Publish\Inventory Tracker New\InventoryTracker\InventoryTracker-WebApp\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
   <si>
     <t>Start Date:</t>
   </si>
@@ -48,6 +48,21 @@
   </si>
   <si>
     <t>EQUIP_TYPE</t>
+  </si>
+  <si>
+    <t>07/14/2023</t>
+  </si>
+  <si>
+    <t>Start Date</t>
+  </si>
+  <si>
+    <t>End Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entity Name </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Start Date </t>
   </si>
 </sst>
 </file>
@@ -412,7 +427,7 @@
   <dimension ref="A1:GV2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -428,7 +443,7 @@
     <col min="9" max="9" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="8.7109375" bestFit="1" customWidth="1"/>
@@ -441,6 +456,12 @@
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="K1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2" spans="1:204" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -471,25 +492,29 @@
         <v>6</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="M2" s="4" t="s">
         <v>4</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
+        <v>10</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="R2" s="4"/>
       <c r="S2" s="4"/>
       <c r="T2" s="4"/>

</xml_diff>